<commit_message>
Changed the way that I get the value from the Sheet and added Java Doc
</commit_message>
<xml_diff>
--- a/src/main/resources/testFile.xlsx
+++ b/src/main/resources/testFile.xlsx
@@ -170,7 +170,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -199,11 +199,16 @@
       <c r="B2" s="0" t="n">
         <v>5678</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="2" t="n">
         <v>12042019</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>